<commit_message>
Envio de email e Finalização do relatorio
</commit_message>
<xml_diff>
--- a/Data/Output/SalesList.xlsx
+++ b/Data/Output/SalesList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinii\OneDrive\Documentos\UiPath\NubankRpaCase\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A17CED-7E1A-409E-BD4B-864204822553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B9C25A-7586-4E97-A059-BFD165D7E50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{340E3889-B257-4942-8996-5EEAB31DBD88}"/>
+    <workbookView xWindow="-20385" yWindow="3210" windowWidth="13605" windowHeight="11295" xr2:uid="{F457EFF8-6654-4062-B107-DF899C573F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="117">
   <si>
     <t>QTY</t>
   </si>
@@ -387,15 +387,6 @@
   </si>
   <si>
     <t>175050 USD</t>
-  </si>
-  <si>
-    <t>Avenida Senador Queirós</t>
-  </si>
-  <si>
-    <t>Centro</t>
-  </si>
-  <si>
-    <t>São Paulo/SP</t>
   </si>
 </sst>
 </file>
@@ -431,11 +422,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,7 +759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8EBF89F-5AA1-4B14-8533-FD3F0829C653}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D4CD9C-25CE-4BEA-A362-AFFCA3E7E5CD}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O30"/>
   <sheetViews>
@@ -901,24 +891,6 @@
       <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="I4">
-        <v>32448.758936000002</v>
-      </c>
-      <c r="J4">
-        <v>162243.79467999999</v>
-      </c>
-      <c r="K4" s="3">
-        <v>46045.253877314812</v>
-      </c>
-      <c r="L4" t="s">
-        <v>117</v>
-      </c>
-      <c r="M4" t="s">
-        <v>118</v>
-      </c>
-      <c r="N4" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">

</xml_diff>